<commit_message>
annual electricity consumption reduced to 1200+
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario.xlsx
+++ b/data/input_behavior/BehaviorScenario.xlsx
@@ -1,32 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yus\Documents\code\3E\FLEX\data\input_behavior\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_behavior/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4014DD18-FB00-CC44-955A-8F0E35246DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="765" windowWidth="30240" windowHeight="17415"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -45,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -402,21 +391,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -427,7 +416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -435,29 +424,95 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>0.6</v>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add person type 4
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario.xlsx
+++ b/data/input_behavior/BehaviorScenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_behavior/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rickm\Documents\Git\Flex\data\input_behavior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4014DD18-FB00-CC44-955A-8F0E35246DC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3901C60D-2054-4A5E-B95D-96675C778DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="710" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -392,20 +392,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="137" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,7 +416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -427,7 +427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -438,7 +438,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -449,7 +449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -460,7 +460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -471,7 +471,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -482,7 +482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -493,7 +493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -504,7 +504,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -512,6 +512,39 @@
         <v>3</v>
       </c>
       <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added a new type of household and added scenarios
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario.xlsx
+++ b/data/input_behavior/BehaviorScenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rickm\Documents\Git\Flex\data\input_behavior\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_behavior/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3901C60D-2054-4A5E-B95D-96675C778DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D4B2DC-FDDA-E44C-8576-FCFB32BC5906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="710" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4340" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -392,20 +392,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="137" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="137" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -416,7 +416,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -427,7 +427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -435,10 +435,10 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -446,105 +446,303 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
         <v>4</v>
       </c>
-      <c r="C13">
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
         <v>1</v>
       </c>
     </row>

</xml_diff>